<commit_message>
Updated OpenCart Test Senarios
</commit_message>
<xml_diff>
--- a/OpenCart-Test Scenarios .xlsx
+++ b/OpenCart-Test Scenarios .xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hemelsarker/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hemelsarker/Documents/GitHub/OpenCart-Manual-Testing-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77B7429-8473-B347-83E4-D19C8DF2B56F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C789CA-370D-4B45-8BF2-4DC4914B3A92}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="84">
   <si>
     <t>Project Name</t>
   </si>
@@ -159,9 +159,6 @@
     <t>OpenCart</t>
   </si>
   <si>
-    <t>Pavan</t>
-  </si>
-  <si>
     <t>Validate the working of Register Account functionality</t>
   </si>
   <si>
@@ -241,6 +238,45 @@
   </si>
   <si>
     <t>DD-MM-YYYY</t>
+  </si>
+  <si>
+    <t>TS_026</t>
+  </si>
+  <si>
+    <t>Validate the working of 'Newsletter' functionality</t>
+  </si>
+  <si>
+    <t>TS_027</t>
+  </si>
+  <si>
+    <t>Validate the working of 'Contact Us' page functionality</t>
+  </si>
+  <si>
+    <t>TS_028</t>
+  </si>
+  <si>
+    <t>Validate the working of 'Gift Certificate' page functionality</t>
+  </si>
+  <si>
+    <t>TS_029</t>
+  </si>
+  <si>
+    <t>Validate the working of 'Speal Offers' page functionality</t>
+  </si>
+  <si>
+    <t>TS_030</t>
+  </si>
+  <si>
+    <t>Validate the working of 'Header' options, 'Menu' options and 'Footer' options</t>
+  </si>
+  <si>
+    <t>TS_031</t>
+  </si>
+  <si>
+    <t>Validate the complete Application functionality for different currencies</t>
+  </si>
+  <si>
+    <t>Hemel</t>
   </si>
 </sst>
 </file>
@@ -390,7 +426,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -428,9 +464,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -442,9 +475,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -735,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -756,55 +786,55 @@
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="20"/>
+      <c r="C2" s="18"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="20"/>
+      <c r="C3" s="18"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="C4" s="20"/>
+      <c r="B4" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="18"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="20"/>
+      <c r="B5" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="18"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6" s="20"/>
+      <c r="B6" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="18"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="C7" s="20"/>
+      <c r="B7" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="18"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
@@ -828,10 +858,10 @@
         <v>11</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>35</v>
@@ -845,10 +875,10 @@
         <v>12</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>35</v>
@@ -862,10 +892,10 @@
         <v>13</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>35</v>
@@ -879,10 +909,10 @@
         <v>14</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>36</v>
@@ -896,10 +926,10 @@
         <v>15</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>37</v>
@@ -913,10 +943,10 @@
         <v>16</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>38</v>
@@ -930,10 +960,10 @@
         <v>17</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>37</v>
@@ -947,10 +977,10 @@
         <v>18</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>37</v>
@@ -964,10 +994,10 @@
         <v>19</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>38</v>
@@ -981,10 +1011,10 @@
         <v>20</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>37</v>
@@ -998,10 +1028,10 @@
         <v>21</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>36</v>
@@ -1015,10 +1045,10 @@
         <v>22</v>
       </c>
       <c r="B22" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="8" t="s">
         <v>69</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>70</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>37</v>
@@ -1032,10 +1062,10 @@
         <v>23</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>36</v>
@@ -1049,10 +1079,10 @@
         <v>24</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>39</v>
@@ -1066,10 +1096,10 @@
         <v>25</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>39</v>
@@ -1083,10 +1113,10 @@
         <v>26</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>39</v>
@@ -1100,10 +1130,10 @@
         <v>27</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>39</v>
@@ -1117,10 +1147,10 @@
         <v>41</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>39</v>
@@ -1134,10 +1164,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>39</v>
@@ -1151,10 +1181,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>39</v>
@@ -1168,10 +1198,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>39</v>
@@ -1185,10 +1215,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>39</v>
@@ -1202,10 +1232,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>39</v>
@@ -1219,10 +1249,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>39</v>
@@ -1236,10 +1266,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>38</v>
@@ -1248,47 +1278,107 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="6"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="9"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="6"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="13"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="14"/>
-      <c r="B38" s="11"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="13"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="15"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="13"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="15"/>
-      <c r="B40" s="16"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="16"/>
-      <c r="E40" s="18"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="15"/>
-      <c r="B41" s="16"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="18"/>
+    <row r="36" spans="1:5" ht="14" x14ac:dyDescent="0.2">
+      <c r="A36" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E36" s="7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="14" x14ac:dyDescent="0.2">
+      <c r="A37" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E37" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="14" x14ac:dyDescent="0.2">
+      <c r="A38" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E38" s="11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="14" x14ac:dyDescent="0.2">
+      <c r="A39" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E39" s="11">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="14" x14ac:dyDescent="0.2">
+      <c r="A40" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E40" s="15">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="14" x14ac:dyDescent="0.2">
+      <c r="A41" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E41" s="15">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Update OpenCart-Test Scenarios .xlsx
</commit_message>
<xml_diff>
--- a/OpenCart-Test Scenarios .xlsx
+++ b/OpenCart-Test Scenarios .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hemelsarker/Documents/GitHub/OpenCart-Manual-Testing-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C789CA-370D-4B45-8BF2-4DC4914B3A92}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D427703C-3FED-E04F-BA05-408C8C3FBF69}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="83">
   <si>
     <t>Project Name</t>
   </si>
@@ -145,9 +145,6 @@
   </si>
   <si>
     <t>P3</t>
-  </si>
-  <si>
-    <t>09</t>
   </si>
   <si>
     <t>TS_018</t>
@@ -765,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:C5"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -787,7 +784,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" s="18"/>
     </row>
@@ -796,7 +793,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" s="18"/>
     </row>
@@ -805,7 +802,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C4" s="18"/>
     </row>
@@ -814,7 +811,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C5" s="18"/>
     </row>
@@ -823,7 +820,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C6" s="18"/>
     </row>
@@ -832,7 +829,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C7" s="18"/>
     </row>
@@ -858,527 +855,465 @@
         <v>11</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="9">
-        <v>27</v>
-      </c>
+      <c r="E11" s="9"/>
     </row>
     <row r="12" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="9">
-        <v>23</v>
-      </c>
+      <c r="E12" s="9"/>
     </row>
     <row r="13" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="9">
-        <v>11</v>
-      </c>
+      <c r="E13" s="9"/>
     </row>
     <row r="14" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="9">
-        <v>25</v>
-      </c>
+      <c r="E14" s="9"/>
     </row>
     <row r="15" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="9">
-        <v>22</v>
-      </c>
+      <c r="E15" s="9"/>
     </row>
     <row r="16" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="9">
-        <v>24</v>
-      </c>
+      <c r="E16" s="9"/>
     </row>
     <row r="17" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="9">
-        <v>37</v>
-      </c>
+      <c r="E17" s="9"/>
     </row>
     <row r="18" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="10" t="s">
-        <v>40</v>
-      </c>
+      <c r="E18" s="10"/>
     </row>
     <row r="19" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="9">
-        <v>21</v>
-      </c>
+      <c r="E19" s="9"/>
     </row>
     <row r="20" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="9">
-        <v>33</v>
-      </c>
+      <c r="E20" s="9"/>
     </row>
     <row r="21" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="9">
-        <v>10</v>
-      </c>
+      <c r="E21" s="9"/>
     </row>
     <row r="22" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="8" t="s">
         <v>68</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>69</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="9">
-        <v>20</v>
-      </c>
+      <c r="E22" s="9"/>
     </row>
     <row r="23" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="9">
-        <v>9</v>
-      </c>
+      <c r="E23" s="9"/>
     </row>
     <row r="24" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E24" s="9">
-        <v>13</v>
-      </c>
+      <c r="E24" s="9"/>
     </row>
     <row r="25" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E25" s="9">
-        <v>13</v>
-      </c>
+      <c r="E25" s="9"/>
     </row>
     <row r="26" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E26" s="9">
-        <v>21</v>
-      </c>
+      <c r="E26" s="9"/>
     </row>
     <row r="27" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E27" s="9">
-        <v>12</v>
-      </c>
+      <c r="E27" s="9"/>
     </row>
     <row r="28" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E28" s="9">
-        <v>8</v>
-      </c>
+      <c r="E28" s="9"/>
     </row>
     <row r="29" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="9">
-        <v>11</v>
-      </c>
+      <c r="E29" s="9"/>
     </row>
     <row r="30" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="9">
-        <v>13</v>
-      </c>
+      <c r="E30" s="9"/>
     </row>
     <row r="31" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E31" s="9">
-        <v>10</v>
-      </c>
+      <c r="E31" s="9"/>
     </row>
     <row r="32" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E32" s="9">
-        <v>17</v>
-      </c>
+      <c r="E32" s="9"/>
     </row>
     <row r="33" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>32</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E33" s="9">
-        <v>11</v>
-      </c>
+      <c r="E33" s="9"/>
     </row>
     <row r="34" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E34" s="9">
-        <v>9</v>
-      </c>
+      <c r="E34" s="9"/>
     </row>
     <row r="35" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E35" s="9">
-        <v>29</v>
-      </c>
+      <c r="E35" s="9"/>
     </row>
     <row r="36" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="8" t="s">
         <v>71</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>72</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E36" s="7">
-        <v>13</v>
-      </c>
+      <c r="E36" s="7"/>
     </row>
     <row r="37" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="12" t="s">
         <v>73</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>74</v>
       </c>
       <c r="D37" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E37" s="11">
-        <v>13</v>
-      </c>
+      <c r="E37" s="11"/>
     </row>
     <row r="38" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A38" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" s="12" t="s">
         <v>75</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>76</v>
       </c>
       <c r="D38" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E38" s="11">
-        <v>11</v>
-      </c>
+      <c r="E38" s="11"/>
     </row>
     <row r="39" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A39" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" s="16" t="s">
         <v>77</v>
-      </c>
-      <c r="B39" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="C39" s="16" t="s">
-        <v>78</v>
       </c>
       <c r="D39" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="E39" s="11">
-        <v>16</v>
-      </c>
+      <c r="E39" s="11"/>
     </row>
     <row r="40" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A40" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40" s="16" t="s">
         <v>79</v>
-      </c>
-      <c r="B40" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="C40" s="16" t="s">
-        <v>80</v>
       </c>
       <c r="D40" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="E40" s="15">
-        <v>22</v>
-      </c>
+      <c r="E40" s="15"/>
     </row>
     <row r="41" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A41" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C41" s="16" t="s">
         <v>81</v>
-      </c>
-      <c r="B41" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="C41" s="16" t="s">
-        <v>82</v>
       </c>
       <c r="D41" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="E41" s="15">
-        <v>3</v>
-      </c>
+      <c r="E41" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1392,8 +1327,5 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="E18" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>